<commit_message>
feat: add seventh lesson, update hour log, README.md, and DataScience image
</commit_message>
<xml_diff>
--- a/Hourlog.xlsx
+++ b/Hourlog.xlsx
@@ -500,7 +500,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -538,7 +538,7 @@
       </c>
       <c r="E2" s="5">
         <f>E1-SUM(B:B)</f>
-        <v>9.5</v>
+        <v>7.5</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>2</v>
@@ -589,6 +589,14 @@
         <v>43034</v>
       </c>
       <c r="B8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="6">
+        <v>43046</v>
+      </c>
+      <c r="B9">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: update hour log
</commit_message>
<xml_diff>
--- a/Hourlog.xlsx
+++ b/Hourlog.xlsx
@@ -46,7 +46,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -116,6 +116,20 @@
       <i/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF008000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
@@ -144,22 +158,31 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -500,108 +523,114 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="10"/>
+    <col min="6" max="6" width="10.83203125" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="3">
+      <c r="E1" s="2">
         <v>20</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="10" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="4">
         <f>E1-SUM(B:B)</f>
-        <v>7.5</v>
-      </c>
-      <c r="F2" s="9" t="s">
+        <v>5.5</v>
+      </c>
+      <c r="F2" s="11" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="6">
+      <c r="A3" s="9">
         <v>43018</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="6">
+      <c r="A4" s="9">
         <v>43020</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="6">
+      <c r="A5" s="9">
         <v>43024</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="6">
+      <c r="A6" s="9">
         <v>43026</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="6">
         <v>1.5</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="6">
+      <c r="A7" s="9">
         <v>43032</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="6">
+      <c r="A8" s="9">
         <v>43034</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="6">
+      <c r="A9" s="9">
         <v>43046</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="C10" s="4"/>
+      <c r="A10" s="9">
+        <v>43048</v>
+      </c>
+      <c r="B10" s="6">
+        <v>2</v>
+      </c>
+      <c r="C10" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
feat: update Hourlog, PythonNotes, TerminalNotes
</commit_message>
<xml_diff>
--- a/Hourlog.xlsx
+++ b/Hourlog.xlsx
@@ -524,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -565,7 +565,7 @@
       </c>
       <c r="E2" s="4">
         <f>E1-SUM(B:B)</f>
-        <v>1.5</v>
+        <v>-0.5</v>
       </c>
       <c r="F2" s="11" t="s">
         <v>2</v>
@@ -649,6 +649,14 @@
         <v>43054</v>
       </c>
       <c r="B12" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="9">
+        <v>43069</v>
+      </c>
+      <c r="B13" s="6">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: add thirteenth lesson and update hourlog
</commit_message>
<xml_diff>
--- a/Hourlog.xlsx
+++ b/Hourlog.xlsx
@@ -524,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -565,7 +565,7 @@
       </c>
       <c r="E2" s="4">
         <f>E1-SUM(B:B)</f>
-        <v>-0.5</v>
+        <v>-4.5</v>
       </c>
       <c r="F2" s="11" t="s">
         <v>2</v>
@@ -657,6 +657,22 @@
         <v>43069</v>
       </c>
       <c r="B13" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="9">
+        <v>43074</v>
+      </c>
+      <c r="B14" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="9">
+        <v>43076</v>
+      </c>
+      <c r="B15" s="6">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: update scraper and add utilities
</commit_message>
<xml_diff>
--- a/Hourlog.xlsx
+++ b/Hourlog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>Tutoring Hour Log</t>
   </si>
@@ -40,6 +40,12 @@
   </si>
   <si>
     <t>DI</t>
+  </si>
+  <si>
+    <t>New Set of Hours</t>
+  </si>
+  <si>
+    <t>Lesson No.</t>
   </si>
 </sst>
 </file>
@@ -52,6 +58,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -524,155 +531,212 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="6"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:7">
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2">
-        <v>20</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="5" t="s">
+      <c r="F1" s="2">
+        <v>40</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="4">
-        <f>E1-SUM(B:B)</f>
-        <v>-4.5</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="9">
+      <c r="F2" s="4">
+        <f>F1-SUM(C:C)</f>
+        <v>13.5</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9">
         <v>43018</v>
       </c>
-      <c r="B3" s="6">
+      <c r="C3" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="9">
+    <row r="4" spans="1:7">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="9">
         <v>43020</v>
       </c>
-      <c r="B4" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="9">
+      <c r="C4" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="9">
         <v>43024</v>
       </c>
-      <c r="B5" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="9">
+      <c r="C5" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="9">
         <v>43026</v>
       </c>
-      <c r="B6" s="6">
+      <c r="C6" s="6">
         <v>1.5</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="9">
+    <row r="7" spans="1:7">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="9">
         <v>43032</v>
       </c>
-      <c r="B7" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="9">
+      <c r="C7" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="9">
         <v>43034</v>
       </c>
-      <c r="B8" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="9">
+      <c r="C8" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="9">
         <v>43046</v>
       </c>
-      <c r="B9" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="9">
+      <c r="C9" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" s="9">
         <v>43048</v>
       </c>
-      <c r="B10" s="6">
-        <v>2</v>
-      </c>
-      <c r="C10" s="3"/>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="9">
+      <c r="C10" s="6">
+        <v>2</v>
+      </c>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" s="9">
         <v>43052</v>
       </c>
-      <c r="B11" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="9">
+      <c r="C11" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" s="9">
         <v>43054</v>
       </c>
-      <c r="B12" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="9">
+      <c r="C12" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" s="9">
         <v>43069</v>
       </c>
-      <c r="B13" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="9">
+      <c r="C13" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" s="9">
         <v>43074</v>
       </c>
-      <c r="B14" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="9">
+      <c r="C14" s="6">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" s="9">
         <v>43076</v>
       </c>
-      <c r="B15" s="6">
+      <c r="C15" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" s="9">
+        <v>43082</v>
+      </c>
+      <c r="C16" s="6">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: add fifteenth lesson
</commit_message>
<xml_diff>
--- a/Hourlog.xlsx
+++ b/Hourlog.xlsx
@@ -531,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="B17" sqref="B17:B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -576,7 +576,7 @@
       </c>
       <c r="F2" s="4">
         <f>F1-SUM(C:C)</f>
-        <v>13.5</v>
+        <v>9.5</v>
       </c>
       <c r="G2" s="11" t="s">
         <v>2</v>
@@ -737,6 +737,28 @@
         <v>43082</v>
       </c>
       <c r="C16" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" s="9">
+        <v>43087</v>
+      </c>
+      <c r="C17" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" s="9">
+        <v>43088</v>
+      </c>
+      <c r="C18" s="6">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: update hourlog and README
</commit_message>
<xml_diff>
--- a/Hourlog.xlsx
+++ b/Hourlog.xlsx
@@ -531,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:B18"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -576,7 +576,7 @@
       </c>
       <c r="F2" s="4">
         <f>F1-SUM(C:C)</f>
-        <v>9.5</v>
+        <v>7.5</v>
       </c>
       <c r="G2" s="11" t="s">
         <v>2</v>
@@ -759,6 +759,17 @@
         <v>43088</v>
       </c>
       <c r="C18" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" s="9">
+        <v>43117</v>
+      </c>
+      <c r="C19" s="6">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: add twentieth lesson
</commit_message>
<xml_diff>
--- a/Hourlog.xlsx
+++ b/Hourlog.xlsx
@@ -542,7 +542,7 @@
   <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -584,7 +584,7 @@
       </c>
       <c r="F2" s="4">
         <f>F1-SUM(C:C)</f>
-        <v>3.5</v>
+        <v>-0.5</v>
       </c>
       <c r="G2" s="11" t="s">
         <v>2</v>
@@ -722,7 +722,7 @@
       <c r="C14" s="6">
         <v>2</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="3" t="s">
         <v>7</v>
       </c>
     </row>
@@ -804,10 +804,26 @@
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="B22" s="6"/>
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" s="9">
+        <v>43136</v>
+      </c>
+      <c r="C22" s="6">
+        <v>2</v>
+      </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="B23" s="6"/>
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23" s="9">
+        <v>43138</v>
+      </c>
+      <c r="C23" s="6">
+        <v>2</v>
+      </c>
     </row>
     <row r="24" spans="1:3">
       <c r="B24" s="6"/>

</xml_diff>

<commit_message>
feat: update README and Hourlog
</commit_message>
<xml_diff>
--- a/Hourlog.xlsx
+++ b/Hourlog.xlsx
@@ -48,7 +48,7 @@
     <t>Lesson No.</t>
   </si>
   <si>
-    <t>END OF PAID HOURS</t>
+    <t>END OF 2nd SET HOURS</t>
   </si>
 </sst>
 </file>
@@ -61,7 +61,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -552,7 +551,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.83203125" style="6"/>
   </cols>
   <sheetData>
@@ -588,7 +587,7 @@
       </c>
       <c r="F2" s="4">
         <f>F1-SUM(C:C)</f>
-        <v>-0.5</v>
+        <v>-2.5</v>
       </c>
       <c r="G2" s="11" t="s">
         <v>2</v>
@@ -833,7 +832,15 @@
       </c>
     </row>
     <row r="24" spans="1:4">
-      <c r="B24" s="6"/>
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24" s="9">
+        <v>43146</v>
+      </c>
+      <c r="C24" s="6">
+        <v>2</v>
+      </c>
     </row>
     <row r="25" spans="1:4">
       <c r="B25" s="6"/>

</xml_diff>